<commit_message>
Fixed vocab URI in exemple 7
</commit_message>
<xml_diff>
--- a/fr.sparna/rdf/skos/skos-play/src/main/webapp/excel_test/excel2skos-exemple-7.xlsx
+++ b/fr.sparna/rdf/skos/skos-play/src/main/webapp/excel_test/excel2skos-exemple-7.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">ConceptScheme URI</t>
   </si>
   <si>
-    <t xml:space="preserve">http://data.sparna.fr/vocabularies/days</t>
+    <t xml:space="preserve">http://data.sparna.fr/vocabularies/paintings</t>
   </si>
   <si>
     <t xml:space="preserve">PREFIX</t>
@@ -101,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -132,12 +132,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -208,7 +202,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -292,21 +286,21 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.0283400809717"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.412955465587"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.82995951417"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.9433198380567"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.2429149797571"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -349,6 +343,9 @@
       <c r="C4" s="1"/>
       <c r="D4" s="0"/>
     </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="0"/>
+    </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>9</v>
@@ -366,6 +363,12 @@
         <v>11</v>
       </c>
       <c r="D8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
@@ -411,8 +414,9 @@
     <row r="20" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="http://fr.dbpedia.org/resource/"/>
-    <hyperlink ref="C3" r:id="rId2" display="http://dbpedia.org/ontology/"/>
+    <hyperlink ref="B1" r:id="rId1" display="http://data.sparna.fr/vocabularies/paintings"/>
+    <hyperlink ref="C2" r:id="rId2" display="http://fr.dbpedia.org/resource/"/>
+    <hyperlink ref="C3" r:id="rId3" display="http://dbpedia.org/ontology/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>